<commit_message>
ajout de google analytics dans le head + erreur noté pour le SEO
</commit_message>
<xml_diff>
--- a/mot clé.xlsx
+++ b/mot clé.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\Projet-N-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372AE6C9-7DD3-41BC-8C8F-33E6FAAF976F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE0DBB3-DEB8-41EC-9060-B9F4F26423A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="90" windowWidth="12255" windowHeight="12660" xr2:uid="{B4101F97-97B2-4DDA-9625-F5A86992B9A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B4101F97-97B2-4DDA-9625-F5A86992B9A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>